<commit_message>
Added xGS Model Data
</commit_message>
<xml_diff>
--- a/ML_Model_Data/Match_Data/team & tourney info.xlsx
+++ b/ML_Model_Data/Match_Data/team & tourney info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbrec\Data_Analysis\Final_Project\Match_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbrec\Data_Analysis\Final_Project\uofm_data_capstone_worldcup\ML_Model_Data\Match_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EFBFB30-11A6-4FD4-B72E-41CCA25B6CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F10D7A1-5ADB-41D2-9E25-346672A2FF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-960" windowWidth="29040" windowHeight="15720" xr2:uid="{369CBB44-0E58-40F0-BAAC-F31677487E5A}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$25:$E$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
   <si>
     <t>Competition</t>
   </si>
@@ -209,9 +208,6 @@
     <t>Costa Rica</t>
   </si>
   <si>
-    <t>Most Recent Tournament</t>
-  </si>
-  <si>
     <t>xGS Standard</t>
   </si>
   <si>
@@ -270,13 +266,34 @@
   </si>
   <si>
     <t>EUFA</t>
+  </si>
+  <si>
+    <t>xGS MISC</t>
+  </si>
+  <si>
+    <t>*CONTAINS MATCHES PLAYED for Team</t>
+  </si>
+  <si>
+    <t>*NOTES</t>
+  </si>
+  <si>
+    <t>the xGS Misc contains team red/yellow card stats - will likely want to switch data</t>
+  </si>
+  <si>
+    <t>2022 EUFA WCQ</t>
+  </si>
+  <si>
+    <t>Most Recent Competition</t>
+  </si>
+  <si>
+    <t>Host</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +312,12 @@
       <color rgb="FF202122"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -638,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2200B4-FF27-4983-B1F8-5FA5DFB6326A}">
-  <dimension ref="B2:J57"/>
+  <dimension ref="B1:N57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,12 +672,24 @@
     <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -662,28 +697,34 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
         <v>57</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" t="s">
         <v>58</v>
       </c>
-      <c r="H2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>59</v>
       </c>
-      <c r="J2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
@@ -695,19 +736,28 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -719,19 +769,28 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -740,22 +799,31 @@
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I5" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -767,19 +835,28 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -791,19 +868,28 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I7" t="s">
+        <v>61</v>
+      </c>
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -815,19 +901,28 @@
         <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
@@ -839,19 +934,28 @@
         <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
@@ -863,19 +967,28 @@
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I10" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
@@ -887,19 +1000,28 @@
         <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
@@ -911,19 +1033,28 @@
         <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
@@ -935,19 +1066,28 @@
         <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I13" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" t="s">
+        <v>61</v>
+      </c>
+      <c r="K13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
@@ -959,19 +1099,28 @@
         <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I14" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
@@ -983,19 +1132,28 @@
         <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" t="s">
+        <v>61</v>
+      </c>
+      <c r="K15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1007,21 +1165,30 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C17">
         <v>2022</v>
@@ -1030,21 +1197,30 @@
         <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18">
         <v>2022</v>
@@ -1053,12 +1229,12 @@
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19">
         <v>2022</v>
@@ -1067,12 +1243,30 @@
         <v>25</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20">
         <v>2022</v>
@@ -1081,12 +1275,12 @@
         <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21">
         <v>2022</v>
@@ -1095,27 +1289,45 @@
         <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22">
         <v>2021</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I22" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" t="s">
+        <v>61</v>
+      </c>
+      <c r="K22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>16</v>
       </c>
@@ -1126,24 +1338,24 @@
         <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>19</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="2">
-        <v>40514</v>
+      <c r="D26" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="E26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -1154,10 +1366,10 @@
         <v>44588</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>36</v>
       </c>
@@ -1167,8 +1379,11 @@
       <c r="D28" s="2">
         <v>44593</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>37</v>
       </c>
@@ -1178,8 +1393,11 @@
       <c r="D29" s="2">
         <v>44644</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>38</v>
       </c>
@@ -1189,8 +1407,11 @@
       <c r="D30" s="2">
         <v>44644</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>54</v>
       </c>
@@ -1200,8 +1421,11 @@
       <c r="D31" s="2">
         <v>44725</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>43</v>
       </c>
@@ -1211,8 +1435,11 @@
       <c r="D32" s="2">
         <v>44649</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -1222,8 +1449,11 @@
       <c r="D33" s="2">
         <v>44649</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>48</v>
       </c>
@@ -1233,8 +1463,11 @@
       <c r="D34" s="2">
         <v>44649</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>49</v>
       </c>
@@ -1244,8 +1477,11 @@
       <c r="D35" s="2">
         <v>44649</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>50</v>
       </c>
@@ -1255,8 +1491,11 @@
       <c r="D36" s="2">
         <v>44649</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>41</v>
       </c>
@@ -1266,8 +1505,11 @@
       <c r="D37" s="2">
         <v>44647</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>51</v>
       </c>
@@ -1277,8 +1519,11 @@
       <c r="D38" s="2">
         <v>44650</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>52</v>
       </c>
@@ -1288,8 +1533,11 @@
       <c r="D39" s="2">
         <v>44650</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>55</v>
       </c>
@@ -1299,8 +1547,11 @@
       <c r="D40" s="2">
         <v>44726</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>24</v>
       </c>
@@ -1310,8 +1561,11 @@
       <c r="D41" s="2">
         <v>44511</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>34</v>
       </c>
@@ -1321,8 +1575,11 @@
       <c r="D42" s="2">
         <v>44516</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>39</v>
       </c>
@@ -1332,8 +1589,11 @@
       <c r="D43" s="2">
         <v>44644</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>40</v>
       </c>
@@ -1343,8 +1603,11 @@
       <c r="D44" s="2">
         <v>44644</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>21</v>
       </c>
@@ -1354,8 +1617,11 @@
       <c r="D45" s="2">
         <v>44480</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>23</v>
       </c>
@@ -1365,8 +1631,11 @@
       <c r="D46" s="2">
         <v>44481</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>26</v>
       </c>
@@ -1376,8 +1645,11 @@
       <c r="D47" s="2">
         <v>44513</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>27</v>
       </c>
@@ -1387,8 +1659,11 @@
       <c r="D48" s="2">
         <v>44513</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>28</v>
       </c>
@@ -1398,8 +1673,11 @@
       <c r="D49" s="2">
         <v>44514</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>29</v>
       </c>
@@ -1409,8 +1687,11 @@
       <c r="D50" s="2">
         <v>44514</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>30</v>
       </c>
@@ -1420,8 +1701,11 @@
       <c r="D51" s="2">
         <v>44514</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>31</v>
       </c>
@@ -1431,8 +1715,11 @@
       <c r="D52" s="2">
         <v>44515</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>32</v>
       </c>
@@ -1442,8 +1729,11 @@
       <c r="D53" s="2">
         <v>44515</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>33</v>
       </c>
@@ -1453,8 +1743,11 @@
       <c r="D54" s="2">
         <v>44516</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>46</v>
       </c>
@@ -1464,8 +1757,11 @@
       <c r="D55" s="2">
         <v>44649</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>47</v>
       </c>
@@ -1475,8 +1771,11 @@
       <c r="D56" s="2">
         <v>44649</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>53</v>
       </c>
@@ -1485,6 +1784,9 @@
       </c>
       <c r="D57" s="2">
         <v>44717</v>
+      </c>
+      <c r="E57" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1493,6 +1795,7 @@
       <sortCondition ref="C25"/>
     </sortState>
   </autoFilter>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>